<commit_message>
More updates to training data
</commit_message>
<xml_diff>
--- a/training_approximate.xlsx
+++ b/training_approximate.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/mixtape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB69B50-9394-DF47-99A6-64B8E276EC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8300E2F2-BEF2-7F43-B6FA-189346937138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37820" yWindow="1280" windowWidth="33960" windowHeight="16940" activeTab="2" xr2:uid="{A3B62EC5-7F5B-6841-B5AB-E336239DA9A2}"/>
+    <workbookView xWindow="-37820" yWindow="1280" windowWidth="33960" windowHeight="16940" activeTab="3" xr2:uid="{A3B62EC5-7F5B-6841-B5AB-E336239DA9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="bias adjustment" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>unit1</t>
   </si>
@@ -1496,7 +1497,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="I3" sqref="I3:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2764,7 +2765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662159BE-45AD-1246-84FC-FA830DE6BF74}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -3400,4 +3401,376 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E2BCE2-55F9-8C46-8EB5-FF2458DB6AC5}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21">
+        <v>18</v>
+      </c>
+      <c r="D2" s="22">
+        <v>1.2768669668126549</v>
+      </c>
+      <c r="E2" s="21">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13">
+        <v>29</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2.8019828173782786</v>
+      </c>
+      <c r="E3" s="13">
+        <v>12250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13">
+        <v>24</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3.9205642309579938</v>
+      </c>
+      <c r="E4" s="13">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13">
+        <v>27</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2.2926678508031757</v>
+      </c>
+      <c r="E5" s="13">
+        <v>11750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13">
+        <v>33</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2.4966702622946206</v>
+      </c>
+      <c r="E6" s="13">
+        <v>13250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13">
+        <v>22</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1.3387078036620916</v>
+      </c>
+      <c r="E7" s="13">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13">
+        <v>7</v>
+      </c>
+      <c r="C8" s="13">
+        <v>19</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1.662759442733091</v>
+      </c>
+      <c r="E8" s="13">
+        <v>9750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>8</v>
+      </c>
+      <c r="C9" s="13">
+        <v>20</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2.598744835539557</v>
+      </c>
+      <c r="E9" s="13">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13">
+        <v>9</v>
+      </c>
+      <c r="C10" s="13">
+        <v>21</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1.9413317247167639</v>
+      </c>
+      <c r="E10" s="13">
+        <v>10250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="17">
+        <v>10</v>
+      </c>
+      <c r="C11" s="17">
+        <v>30</v>
+      </c>
+      <c r="D11" s="18">
+        <v>3.3740289080760242</v>
+      </c>
+      <c r="E11" s="17">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" s="20">
+        <v>13</v>
+      </c>
+      <c r="C12" s="21">
+        <v>22</v>
+      </c>
+      <c r="D12" s="22">
+        <v>1.662291385973246</v>
+      </c>
+      <c r="E12" s="23">
+        <v>8950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" s="12">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13">
+        <v>38</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1.6145408563338297</v>
+      </c>
+      <c r="E13" s="15">
+        <v>12550</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" s="12">
+        <v>8</v>
+      </c>
+      <c r="C14" s="13">
+        <v>33</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1.9747705998072842</v>
+      </c>
+      <c r="E14" s="15">
+        <v>11425</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" s="12">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13">
+        <v>27</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1.77610720900872</v>
+      </c>
+      <c r="E15" s="15">
+        <v>10075</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" s="12">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13">
+        <v>33</v>
+      </c>
+      <c r="D16" s="14">
+        <v>1.9747705998072842</v>
+      </c>
+      <c r="E16" s="15">
+        <v>11425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12">
+        <v>13</v>
+      </c>
+      <c r="C17" s="13">
+        <v>22</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1.662291385973246</v>
+      </c>
+      <c r="E17" s="15">
+        <v>8950</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" s="12">
+        <v>17</v>
+      </c>
+      <c r="C18" s="13">
+        <v>19</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1.8595863891608966</v>
+      </c>
+      <c r="E18" s="15">
+        <v>8275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13">
+        <v>20</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1.8904439599777811</v>
+      </c>
+      <c r="E19" s="15">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="12">
+        <v>3</v>
+      </c>
+      <c r="C20" s="13">
+        <v>21</v>
+      </c>
+      <c r="D20" s="14">
+        <v>1.837511566218393</v>
+      </c>
+      <c r="E20" s="15">
+        <v>8725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" s="16">
+        <v>10</v>
+      </c>
+      <c r="C21" s="17">
+        <v>30</v>
+      </c>
+      <c r="D21" s="18">
+        <v>2.0152083863823114</v>
+      </c>
+      <c r="E21" s="19">
+        <v>10750</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changing up the files
</commit_message>
<xml_diff>
--- a/training_approximate.xlsx
+++ b/training_approximate.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/mixtape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8300E2F2-BEF2-7F43-B6FA-189346937138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16731CE7-AA09-734F-9009-B36B6950AF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37820" yWindow="1280" windowWidth="33960" windowHeight="16940" activeTab="3" xr2:uid="{A3B62EC5-7F5B-6841-B5AB-E336239DA9A2}"/>
+    <workbookView xWindow="-37820" yWindow="1280" windowWidth="33960" windowHeight="16940" activeTab="4" xr2:uid="{A3B62EC5-7F5B-6841-B5AB-E336239DA9A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="bias adjustment" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="bias adjustment" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>unit1</t>
   </si>
@@ -144,6 +145,9 @@
   </si>
   <si>
     <t>earnings</t>
+  </si>
+  <si>
+    <t>naynum11</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1501,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:L12"/>
+      <selection activeCell="I12" sqref="I12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1671,17 +1675,17 @@
       <c r="H3" s="23">
         <v>8500</v>
       </c>
-      <c r="I3" s="20">
-        <v>13</v>
-      </c>
-      <c r="J3" s="21">
-        <v>22</v>
-      </c>
-      <c r="K3" s="22">
-        <v>1.662291385973246</v>
-      </c>
-      <c r="L3" s="23">
-        <v>8950</v>
+      <c r="I3" s="12">
+        <v>14</v>
+      </c>
+      <c r="J3" s="13">
+        <v>18</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1.89</v>
+      </c>
+      <c r="L3" s="15">
+        <v>8050</v>
       </c>
       <c r="M3" s="20">
         <v>4</v>
@@ -1709,11 +1713,11 @@
       </c>
       <c r="U3" s="20">
         <f>(B3-J3)^2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="V3" s="23">
         <f>(C3-K3)^2</f>
-        <v>0.14855198288527904</v>
+        <v>0.37593211638551394</v>
       </c>
       <c r="W3" s="20">
         <f>(B3-N3)^2</f>
@@ -1758,16 +1762,16 @@
         <v>10075</v>
       </c>
       <c r="I4" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J4" s="13">
-        <v>38</v>
-      </c>
-      <c r="K4" s="14">
-        <v>1.6145408563338297</v>
+        <v>29</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1.74</v>
       </c>
       <c r="L4" s="15">
-        <v>12550</v>
+        <v>10525</v>
       </c>
       <c r="M4" s="12">
         <v>20</v>
@@ -1795,11 +1799,11 @@
       </c>
       <c r="U4" s="12">
         <f>(B4-J4)^2</f>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="V4" s="15">
         <f>(C4-K4)^2</f>
-        <v>1.4100184108490865</v>
+        <v>1.1278075044067062</v>
       </c>
       <c r="W4" s="12">
         <f>(B4-N4)^2</f>
@@ -1844,16 +1848,16 @@
         <v>8725</v>
       </c>
       <c r="I5" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J5" s="13">
-        <v>33</v>
-      </c>
-      <c r="K5" s="14">
-        <v>1.9747705998072842</v>
+        <v>24</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1.81</v>
       </c>
       <c r="L5" s="15">
-        <v>11425</v>
+        <v>9400</v>
       </c>
       <c r="M5" s="12">
         <v>12</v>
@@ -1881,11 +1885,11 @@
       </c>
       <c r="U5" s="12">
         <f>(B5-J5)^2</f>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="V5" s="15">
         <f>(C5-K5)^2</f>
-        <v>3.7861128550266638</v>
+        <v>4.4544813729993074</v>
       </c>
       <c r="W5" s="12">
         <f>(B5-N5)^2</f>
@@ -1935,8 +1939,8 @@
       <c r="J6" s="13">
         <v>27</v>
       </c>
-      <c r="K6" s="14">
-        <v>1.77610720900872</v>
+      <c r="K6" s="13">
+        <v>1.78</v>
       </c>
       <c r="L6" s="15">
         <v>10075</v>
@@ -1971,7 +1975,7 @@
       </c>
       <c r="V6" s="15">
         <f>(C6-K6)^2</f>
-        <v>0.2668348966511</v>
+        <v>0.26282832524714717</v>
       </c>
       <c r="W6" s="12">
         <f>(B6-N6)^2</f>
@@ -2021,8 +2025,8 @@
       <c r="J7" s="13">
         <v>33</v>
       </c>
-      <c r="K7" s="14">
-        <v>1.9747705998072842</v>
+      <c r="K7" s="13">
+        <v>1.97</v>
       </c>
       <c r="L7" s="15">
         <v>11425</v>
@@ -2057,7 +2061,7 @@
       </c>
       <c r="V7" s="15">
         <f>(C7-K7)^2</f>
-        <v>0.27237925770439569</v>
+        <v>0.27738156518548451</v>
       </c>
       <c r="W7" s="12">
         <f>(B7-N7)^2</f>
@@ -2107,8 +2111,8 @@
       <c r="J8" s="13">
         <v>22</v>
       </c>
-      <c r="K8" s="14">
-        <v>1.662291385973246</v>
+      <c r="K8" s="13">
+        <v>1.66</v>
       </c>
       <c r="L8" s="15">
         <v>8950</v>
@@ -2143,7 +2147,7 @@
       </c>
       <c r="V8" s="15">
         <f>(C8-K8)^2</f>
-        <v>0.10470633474131961</v>
+        <v>0.103228675427637</v>
       </c>
       <c r="W8" s="12">
         <f>(B8-N8)^2</f>
@@ -2193,8 +2197,8 @@
       <c r="J9" s="13">
         <v>19</v>
       </c>
-      <c r="K9" s="14">
-        <v>1.8595863891608966</v>
+      <c r="K9" s="13">
+        <v>1.86</v>
       </c>
       <c r="L9" s="15">
         <v>8275</v>
@@ -2229,7 +2233,7 @@
       </c>
       <c r="V9" s="15">
         <f>(C9-K9)^2</f>
-        <v>3.8740846840094267E-2</v>
+        <v>3.8903837430960868E-2</v>
       </c>
       <c r="W9" s="12">
         <f>(B9-N9)^2</f>
@@ -2274,16 +2278,16 @@
         <v>11425</v>
       </c>
       <c r="I10" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="13">
-        <v>20</v>
-      </c>
-      <c r="K10" s="14">
-        <v>1.8904439599777811</v>
+        <v>27</v>
+      </c>
+      <c r="K10" s="13">
+        <v>1.78</v>
       </c>
       <c r="L10" s="15">
-        <v>8500</v>
+        <v>10075</v>
       </c>
       <c r="M10" s="12">
         <v>7</v>
@@ -2311,11 +2315,11 @@
       </c>
       <c r="U10" s="12">
         <f>(B10-J10)^2</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="V10" s="15">
         <f>(C10-K10)^2</f>
-        <v>0.50169013032157839</v>
+        <v>0.67034310572269629</v>
       </c>
       <c r="W10" s="12">
         <f>(B10-N10)^2</f>
@@ -2365,8 +2369,8 @@
       <c r="J11" s="13">
         <v>21</v>
       </c>
-      <c r="K11" s="14">
-        <v>1.837511566218393</v>
+      <c r="K11" s="13">
+        <v>1.84</v>
       </c>
       <c r="L11" s="15">
         <v>8725</v>
@@ -2401,7 +2405,7 @@
       </c>
       <c r="V11" s="15">
         <f>(C11-K11)^2</f>
-        <v>1.0778625310626854E-2</v>
+        <v>1.0268118434073993E-2</v>
       </c>
       <c r="W11" s="12">
         <f>(B11-N11)^2</f>
@@ -2451,8 +2455,8 @@
       <c r="J12" s="17">
         <v>30</v>
       </c>
-      <c r="K12" s="18">
-        <v>2.0152083863823114</v>
+      <c r="K12" s="17">
+        <v>2.02</v>
       </c>
       <c r="L12" s="19">
         <v>10750</v>
@@ -2487,7 +2491,7 @@
       </c>
       <c r="V12" s="19">
         <f>(C12-K12)^2</f>
-        <v>1.8463932101759739</v>
+        <v>1.8333942839055504</v>
       </c>
       <c r="W12" s="16">
         <f>(B12-N12)^2</f>
@@ -2532,11 +2536,11 @@
       </c>
       <c r="J13">
         <f>_xlfn.VAR.P(J3:J12)</f>
-        <v>39.85</v>
+        <v>22.4</v>
       </c>
       <c r="K13" s="1">
         <f>_xlfn.VAR.P(K3:K12)</f>
-        <v>1.8627840397090679E-2</v>
+        <v>1.0245000000000001E-2</v>
       </c>
       <c r="N13">
         <f>_xlfn.VAR.P(N3:N12)</f>
@@ -2559,7 +2563,7 @@
       </c>
       <c r="V13" s="19">
         <f>SUM(U3:V12)</f>
-        <v>186.38620655050607</v>
+        <v>58.154568905145076</v>
       </c>
       <c r="W13" s="28" t="s">
         <v>26</v>
@@ -2711,7 +2715,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f>SQRT(V13)</f>
-        <v>13.652333373841486</v>
+        <v>7.6259142996197564</v>
       </c>
       <c r="C26"/>
       <c r="E26" s="1"/>
@@ -2762,6 +2766,863 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB576F-07AE-9345-9BCA-5BFB12B54D5D}">
+  <dimension ref="A2:L38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>1.28</v>
+      </c>
+      <c r="F4">
+        <v>9500</v>
+      </c>
+      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="I4">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>1.89</v>
+      </c>
+      <c r="L4">
+        <v>8050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>2.8</v>
+      </c>
+      <c r="F5">
+        <v>12250</v>
+      </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <v>1.74</v>
+      </c>
+      <c r="L5">
+        <v>10525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>3.92</v>
+      </c>
+      <c r="F6">
+        <v>11000</v>
+      </c>
+      <c r="G6">
+        <v>19</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>1.81</v>
+      </c>
+      <c r="L6">
+        <v>9400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>2.29</v>
+      </c>
+      <c r="F7">
+        <v>11750</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>27</v>
+      </c>
+      <c r="K7">
+        <v>1.78</v>
+      </c>
+      <c r="L7">
+        <v>10075</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>2.5</v>
+      </c>
+      <c r="F8">
+        <v>13250</v>
+      </c>
+      <c r="G8">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>33</v>
+      </c>
+      <c r="K8">
+        <v>1.97</v>
+      </c>
+      <c r="L8">
+        <v>11425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>1.34</v>
+      </c>
+      <c r="F10">
+        <v>10500</v>
+      </c>
+      <c r="G10">
+        <v>23</v>
+      </c>
+      <c r="I10">
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <v>22</v>
+      </c>
+      <c r="K10">
+        <v>1.66</v>
+      </c>
+      <c r="L10">
+        <v>8950</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>1.66</v>
+      </c>
+      <c r="F11">
+        <v>9750</v>
+      </c>
+      <c r="G11">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <v>17</v>
+      </c>
+      <c r="J11">
+        <v>19</v>
+      </c>
+      <c r="K11">
+        <v>1.86</v>
+      </c>
+      <c r="L11">
+        <v>8275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>2.6</v>
+      </c>
+      <c r="F12">
+        <v>10000</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>27</v>
+      </c>
+      <c r="K12">
+        <v>1.78</v>
+      </c>
+      <c r="L12">
+        <v>10075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>1.94</v>
+      </c>
+      <c r="F13">
+        <v>10250</v>
+      </c>
+      <c r="G13">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>21</v>
+      </c>
+      <c r="K13">
+        <v>1.84</v>
+      </c>
+      <c r="L13">
+        <v>8725</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>3.37</v>
+      </c>
+      <c r="F14">
+        <v>12500</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>30</v>
+      </c>
+      <c r="K14">
+        <v>2.02</v>
+      </c>
+      <c r="L14">
+        <v>10750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>1.89</v>
+      </c>
+      <c r="F16">
+        <v>8500</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>1.78</v>
+      </c>
+      <c r="F17">
+        <v>10075</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <v>1.84</v>
+      </c>
+      <c r="F18">
+        <v>8725</v>
+      </c>
+      <c r="G18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>1.76</v>
+      </c>
+      <c r="F19">
+        <v>12775</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>1.61</v>
+      </c>
+      <c r="F20">
+        <v>12550</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>29</v>
+      </c>
+      <c r="E22">
+        <v>1.74</v>
+      </c>
+      <c r="F22">
+        <v>10525</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>1.57</v>
+      </c>
+      <c r="F23">
+        <v>12775</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <v>1.97</v>
+      </c>
+      <c r="F24">
+        <v>11425</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>1.81</v>
+      </c>
+      <c r="F25">
+        <v>9400</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>2.02</v>
+      </c>
+      <c r="F26">
+        <v>10750</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>33</v>
+      </c>
+      <c r="E28">
+        <v>1.64</v>
+      </c>
+      <c r="F28">
+        <v>11425</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>1.7</v>
+      </c>
+      <c r="F29">
+        <v>12100</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <v>1.66</v>
+      </c>
+      <c r="F30">
+        <v>8950</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>1.89</v>
+      </c>
+      <c r="F31">
+        <v>8050</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>43</v>
+      </c>
+      <c r="E32">
+        <v>1.45</v>
+      </c>
+      <c r="F32">
+        <v>13675</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>39</v>
+      </c>
+      <c r="E34">
+        <v>1.88</v>
+      </c>
+      <c r="F34">
+        <v>12775</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>17</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <v>1.86</v>
+      </c>
+      <c r="F35">
+        <v>8275</v>
+      </c>
+      <c r="G35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>30</v>
+      </c>
+      <c r="E36">
+        <v>1.86</v>
+      </c>
+      <c r="F36">
+        <v>9000</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>19</v>
+      </c>
+      <c r="D37">
+        <v>51</v>
+      </c>
+      <c r="E37">
+        <v>1.96</v>
+      </c>
+      <c r="F37">
+        <v>15475</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>48</v>
+      </c>
+      <c r="E38">
+        <v>1.87</v>
+      </c>
+      <c r="F38">
+        <v>14800</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662159BE-45AD-1246-84FC-FA830DE6BF74}">
   <dimension ref="A1:F32"/>
   <sheetViews>
@@ -3403,12 +4264,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E2BCE2-55F9-8C46-8EB5-FF2458DB6AC5}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B17" sqref="B17:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3604,67 +4465,67 @@
       <c r="A12">
         <v>0</v>
       </c>
-      <c r="B12" s="20">
-        <v>13</v>
-      </c>
-      <c r="C12" s="21">
-        <v>22</v>
-      </c>
-      <c r="D12" s="22">
-        <v>1.662291385973246</v>
-      </c>
-      <c r="E12" s="23">
-        <v>8950</v>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1.89</v>
+      </c>
+      <c r="E12">
+        <v>8050</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
-      <c r="B13" s="12">
-        <v>5</v>
-      </c>
-      <c r="C13" s="13">
-        <v>38</v>
-      </c>
-      <c r="D13" s="14">
-        <v>1.6145408563338297</v>
-      </c>
-      <c r="E13" s="15">
-        <v>12550</v>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>1.74</v>
+      </c>
+      <c r="E13">
+        <v>10525</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
-      <c r="B14" s="12">
-        <v>8</v>
-      </c>
-      <c r="C14" s="13">
-        <v>33</v>
-      </c>
-      <c r="D14" s="14">
-        <v>1.9747705998072842</v>
-      </c>
-      <c r="E14" s="15">
-        <v>11425</v>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>1.81</v>
+      </c>
+      <c r="E14">
+        <v>9400</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15">
         <v>27</v>
       </c>
-      <c r="D15" s="14">
-        <v>1.77610720900872</v>
-      </c>
-      <c r="E15" s="15">
+      <c r="D15">
+        <v>1.78</v>
+      </c>
+      <c r="E15">
         <v>10075</v>
       </c>
     </row>
@@ -3672,16 +4533,16 @@
       <c r="A16">
         <v>0</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16">
         <v>8</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16">
         <v>33</v>
       </c>
-      <c r="D16" s="14">
-        <v>1.9747705998072842</v>
-      </c>
-      <c r="E16" s="15">
+      <c r="D16">
+        <v>1.97</v>
+      </c>
+      <c r="E16">
         <v>11425</v>
       </c>
     </row>
@@ -3689,16 +4550,16 @@
       <c r="A17">
         <v>0</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17">
         <v>13</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17">
         <v>22</v>
       </c>
-      <c r="D17" s="14">
-        <v>1.662291385973246</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="D17">
+        <v>1.66</v>
+      </c>
+      <c r="E17">
         <v>8950</v>
       </c>
     </row>
@@ -3706,16 +4567,16 @@
       <c r="A18">
         <v>0</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18">
         <v>19</v>
       </c>
-      <c r="D18" s="14">
-        <v>1.8595863891608966</v>
-      </c>
-      <c r="E18" s="15">
+      <c r="D18">
+        <v>1.86</v>
+      </c>
+      <c r="E18">
         <v>8275</v>
       </c>
     </row>
@@ -3723,50 +4584,50 @@
       <c r="A19">
         <v>0</v>
       </c>
-      <c r="B19" s="12">
-        <v>1</v>
-      </c>
-      <c r="C19" s="13">
-        <v>20</v>
-      </c>
-      <c r="D19" s="14">
-        <v>1.8904439599777811</v>
-      </c>
-      <c r="E19" s="15">
-        <v>8500</v>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>1.78</v>
+      </c>
+      <c r="E19">
+        <v>10075</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20">
         <v>21</v>
       </c>
-      <c r="D20" s="14">
-        <v>1.837511566218393</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="D20">
+        <v>1.84</v>
+      </c>
+      <c r="E20">
         <v>8725</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21">
         <v>10</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21">
         <v>30</v>
       </c>
-      <c r="D21" s="18">
-        <v>2.0152083863823114</v>
-      </c>
-      <c r="E21" s="19">
+      <c r="D21">
+        <v>2.02</v>
+      </c>
+      <c r="E21">
         <v>10750</v>
       </c>
     </row>

</xml_diff>